<commit_message>
update: Thai_Basic.xlsx 파일 업데이트
</commit_message>
<xml_diff>
--- a/public/Thai_Basic.xlsx
+++ b/public/Thai_Basic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Book pro2\Desktop\develop\Thai Language\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333C4E2E-DE2F-4874-B89D-9A4EDA3A336D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834B6140-3AA3-4B92-BCFB-9E9000980836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{50E21768-2997-4E9D-9C7F-B0EC34E93FFF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{50E21768-2997-4E9D-9C7F-B0EC34E93FFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1776" uniqueCount="1161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1905" uniqueCount="1290">
   <si>
     <t>한국어</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2535,9 +2535,42 @@
     <t>미안합니다</t>
   </si>
   <si>
+    <t>책</t>
+  </si>
+  <si>
+    <t>หนังสือ</t>
+  </si>
+  <si>
+    <t>돈</t>
+  </si>
+  <si>
+    <t>เงิน</t>
+  </si>
+  <si>
+    <t>의자</t>
+  </si>
+  <si>
+    <t>เก้าอี้</t>
+  </si>
+  <si>
+    <t>โต๊ะ</t>
+  </si>
+  <si>
+    <t>가방</t>
+  </si>
+  <si>
+    <t>กระเป๋า</t>
+  </si>
+  <si>
     <t>ผม</t>
   </si>
   <si>
+    <t>덥다</t>
+  </si>
+  <si>
+    <t>ร้อน</t>
+  </si>
+  <si>
     <t>듣다</t>
   </si>
   <si>
@@ -2557,6 +2590,27 @@
   </si>
   <si>
     <t>한국어</t>
+  </si>
+  <si>
+    <t>เข้าใจ</t>
+  </si>
+  <si>
+    <t>여기</t>
+  </si>
+  <si>
+    <t>ที่นี่</t>
+  </si>
+  <si>
+    <t>거기</t>
+  </si>
+  <si>
+    <t>ที่นั่น</t>
+  </si>
+  <si>
+    <t>เย็น</t>
+  </si>
+  <si>
+    <t>เข้า</t>
   </si>
   <si>
     <t>쿤 뻰 크라이 크랍</t>
@@ -3970,6 +4024,21 @@
     <t>일본어</t>
   </si>
   <si>
+    <r>
+      <t>파-싸v아 이^-뿐</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>⬊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>파-싸v아 까올리v-</t>
   </si>
   <si>
@@ -3979,9 +4048,6 @@
     <t>파-싸v아 찐-</t>
   </si>
   <si>
-    <t>독일러</t>
-  </si>
-  <si>
     <t>색(색깔)</t>
   </si>
   <si>
@@ -4063,9 +4129,6 @@
     <t>ภาษาอังกฤษ</t>
   </si>
   <si>
-    <t>파-싸v아 이^-뿐⬊</t>
-  </si>
-  <si>
     <t>ภาษาญี่ปุ่น</t>
   </si>
   <si>
@@ -4082,9 +4145,6 @@
   </si>
   <si>
     <t>ภาษาจีน</t>
-  </si>
-  <si>
-    <t>파-싸v아 여라⬈만</t>
   </si>
   <si>
     <t>ภาษาเยอรมัน</t>
@@ -4152,12 +4212,410 @@
     <t>0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>독일어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분홍색</t>
+  </si>
+  <si>
+    <t>씨v- 촘푸-</t>
+  </si>
+  <si>
+    <t>금색</t>
+  </si>
+  <si>
+    <t>씨v- 터엉-</t>
+  </si>
+  <si>
+    <t>은색</t>
+  </si>
+  <si>
+    <t>씨v- 응언</t>
+  </si>
+  <si>
+    <t>응언</t>
+  </si>
+  <si>
+    <t>노란색</t>
+  </si>
+  <si>
+    <t>씨v- 르v앙</t>
+  </si>
+  <si>
+    <t>회색</t>
+  </si>
+  <si>
+    <t>씨v- 타오</t>
+  </si>
+  <si>
+    <t>진한 회색</t>
+  </si>
+  <si>
+    <t>연한 ~색</t>
+  </si>
+  <si>
+    <t>진한 ~색</t>
+  </si>
+  <si>
+    <t>연한 분홍색</t>
+  </si>
+  <si>
+    <r>
+      <t>파-싸v아 여라</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>⬈</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>만</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낭v쓰v으</t>
+  </si>
+  <si>
+    <t>공책</t>
+  </si>
+  <si>
+    <t>탁자</t>
+  </si>
+  <si>
+    <r>
+      <t>또</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>⬈</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>종이</t>
+  </si>
+  <si>
+    <t>안</t>
+  </si>
+  <si>
+    <t>레^앰</t>
+  </si>
+  <si>
+    <t>สีชมพู</t>
+  </si>
+  <si>
+    <t>สีทอง</t>
+  </si>
+  <si>
+    <t>สีเงิน</t>
+  </si>
+  <si>
+    <t>สีเหลือง</t>
+  </si>
+  <si>
+    <t>สีเทา</t>
+  </si>
+  <si>
+    <t>씨v- 깨⬊-</t>
+  </si>
+  <si>
+    <t>สีเข้ม</t>
+  </si>
+  <si>
+    <t>씨v- 타오 깨⬊-</t>
+  </si>
+  <si>
+    <t>สีเทาเข้ม</t>
+  </si>
+  <si>
+    <t>씨v- 어⬊언</t>
+  </si>
+  <si>
+    <t>สีอ่อน</t>
+  </si>
+  <si>
+    <t>씨v- 촘푸-어⬊언</t>
+  </si>
+  <si>
+    <t>สีชมพูอ่อน</t>
+  </si>
+  <si>
+    <t>자 (ruler)</t>
+  </si>
+  <si>
+    <t>마⬈이 반탓⬈</t>
+  </si>
+  <si>
+    <t>ไม้บรรทัด</t>
+  </si>
+  <si>
+    <t>싸⬊뭇⬊</t>
+  </si>
+  <si>
+    <t>สมุด</t>
+  </si>
+  <si>
+    <t>까^오이^이</t>
+  </si>
+  <si>
+    <t>끄라⬊다⬊앗</t>
+  </si>
+  <si>
+    <t>กระดาษ</t>
+  </si>
+  <si>
+    <t>끄라⬊빠v오</t>
+  </si>
+  <si>
+    <t>몇 (숫자)</t>
+  </si>
+  <si>
+    <t>กี่</t>
+  </si>
+  <si>
+    <t>개 (물건 숫자)</t>
+  </si>
+  <si>
+    <t>อัน</t>
+  </si>
+  <si>
+    <t>권 (책)</t>
+  </si>
+  <si>
+    <t>เล่ม</t>
+  </si>
+  <si>
+    <t>장 (종이)</t>
+  </si>
+  <si>
+    <t>패⬊앤</t>
+  </si>
+  <si>
+    <t>แผ่น</t>
+  </si>
+  <si>
+    <t>동물</t>
+  </si>
+  <si>
+    <r>
+      <t>끼</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>⬊</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사람</t>
+  </si>
+  <si>
+    <t>학생</t>
+  </si>
+  <si>
+    <t>남자</t>
+  </si>
+  <si>
+    <t>푸^우 차-이</t>
+  </si>
+  <si>
+    <t>여자</t>
+  </si>
+  <si>
+    <t>아시아인</t>
+  </si>
+  <si>
+    <t>콘 에-치-아</t>
+  </si>
+  <si>
+    <t>서양인</t>
+  </si>
+  <si>
+    <t>저기</t>
+  </si>
+  <si>
+    <t>카^오 짜이</t>
+  </si>
+  <si>
+    <t>들어가다</t>
+  </si>
+  <si>
+    <t>마음</t>
+  </si>
+  <si>
+    <t>짜이</t>
+  </si>
+  <si>
+    <t>배고프다</t>
+  </si>
+  <si>
+    <t>시원하다</t>
+  </si>
+  <si>
+    <t>옌</t>
+  </si>
+  <si>
+    <t>~아니다</t>
+  </si>
+  <si>
+    <t>~마^이</t>
+  </si>
+  <si>
+    <t>~이다</t>
+  </si>
+  <si>
+    <t>뺀~</t>
+  </si>
+  <si>
+    <t>요구하다</t>
+  </si>
+  <si>
+    <t>커v어</t>
+  </si>
+  <si>
+    <t>~좀 주세요</t>
+  </si>
+  <si>
+    <t>여기 있습니다</t>
+  </si>
+  <si>
+    <t>더~</t>
+  </si>
+  <si>
+    <t>쌌⬊ (짧게 발음)</t>
+  </si>
+  <si>
+    <t>สัตว์</t>
+  </si>
+  <si>
+    <t>콘 (짧게)</t>
+  </si>
+  <si>
+    <t>คน</t>
+  </si>
+  <si>
+    <t>나끄⬈리안</t>
+  </si>
+  <si>
+    <t>นักเรียน</t>
+  </si>
+  <si>
+    <t>ผู้ชาย</t>
+  </si>
+  <si>
+    <t>푸^우 잉v (짧게)</t>
+  </si>
+  <si>
+    <t>ผู้หญิง</t>
+  </si>
+  <si>
+    <t>คนเอเชีย</t>
+  </si>
+  <si>
+    <t>퐈 (f발음)⬊랑⬊</t>
+  </si>
+  <si>
+    <t>ฝรั่ง</t>
+  </si>
+  <si>
+    <t>티^이 니^이 (길게)</t>
+  </si>
+  <si>
+    <t>티^이 난^ (짧게)</t>
+  </si>
+  <si>
+    <t>티^이 노^온 (길게)</t>
+  </si>
+  <si>
+    <t>ที่นู่น</t>
+  </si>
+  <si>
+    <t>이해하다 (마음속으로 들어가다)</t>
+  </si>
+  <si>
+    <t>카^오</t>
+  </si>
+  <si>
+    <t>ใจ</t>
+  </si>
+  <si>
+    <t>히v우 (짧게)</t>
+  </si>
+  <si>
+    <t>หิว</t>
+  </si>
+  <si>
+    <t>러⬈언</t>
+  </si>
+  <si>
+    <t>ไม่~</t>
+  </si>
+  <si>
+    <t>เป็น~</t>
+  </si>
+  <si>
+    <t>ขอ</t>
+  </si>
+  <si>
+    <t>커v어 ~ 너⬊-이</t>
+  </si>
+  <si>
+    <t>ขอ ~ หน่อย</t>
+  </si>
+  <si>
+    <t>니^이 크⬈랍</t>
+  </si>
+  <si>
+    <t>นี่ครับ</t>
+  </si>
+  <si>
+    <t>익⬊- (길게)</t>
+  </si>
+  <si>
+    <t>ยิ่ง~</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4180,13 +4638,6 @@
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4226,7 +4677,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4243,9 +4694,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -4567,8 +5015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA52BE45-9FDD-4C11-88B2-8B333C39B087}">
   <dimension ref="A1:N595"/>
   <sheetViews>
-    <sheetView topLeftCell="A528" workbookViewId="0">
-      <selection activeCell="H543" sqref="H543"/>
+    <sheetView tabSelected="1" topLeftCell="A543" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -10253,16 +10701,16 @@
         <v>431</v>
       </c>
       <c r="B432" t="s">
-        <v>690</v>
+        <v>708</v>
       </c>
       <c r="C432" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D432" s="2" t="s">
-        <v>688</v>
+        <v>706</v>
       </c>
       <c r="E432" s="2" t="s">
-        <v>702</v>
+        <v>720</v>
       </c>
     </row>
     <row r="433" spans="1:14" x14ac:dyDescent="0.3">
@@ -10273,10 +10721,10 @@
         <v>6</v>
       </c>
       <c r="D433" s="2" t="s">
-        <v>689</v>
+        <v>707</v>
       </c>
       <c r="E433" s="2" t="s">
-        <v>703</v>
+        <v>721</v>
       </c>
     </row>
     <row r="434" spans="1:14" x14ac:dyDescent="0.3">
@@ -10284,16 +10732,16 @@
         <v>433</v>
       </c>
       <c r="B434" t="s">
-        <v>992</v>
+        <v>1010</v>
       </c>
       <c r="C434" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D434" s="2" t="s">
-        <v>691</v>
+        <v>709</v>
       </c>
       <c r="E434" s="2" t="s">
-        <v>704</v>
+        <v>722</v>
       </c>
     </row>
     <row r="435" spans="1:14" x14ac:dyDescent="0.3">
@@ -10304,10 +10752,10 @@
         <v>6</v>
       </c>
       <c r="D435" s="2" t="s">
-        <v>692</v>
+        <v>710</v>
       </c>
       <c r="E435" s="2" t="s">
-        <v>705</v>
+        <v>723</v>
       </c>
       <c r="K435" s="2"/>
       <c r="L435" s="2"/>
@@ -10319,16 +10767,16 @@
         <v>435</v>
       </c>
       <c r="B436" t="s">
-        <v>693</v>
+        <v>711</v>
       </c>
       <c r="C436" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D436" s="2" t="s">
-        <v>694</v>
+        <v>712</v>
       </c>
       <c r="E436" s="2" t="s">
-        <v>706</v>
+        <v>724</v>
       </c>
       <c r="K436" s="2"/>
       <c r="L436" s="2"/>
@@ -10343,10 +10791,10 @@
         <v>6</v>
       </c>
       <c r="D437" s="2" t="s">
-        <v>695</v>
+        <v>713</v>
       </c>
       <c r="E437" s="2" t="s">
-        <v>707</v>
+        <v>725</v>
       </c>
       <c r="K437" s="2"/>
       <c r="L437" s="2"/>
@@ -10358,16 +10806,16 @@
         <v>437</v>
       </c>
       <c r="B438" t="s">
-        <v>696</v>
+        <v>714</v>
       </c>
       <c r="C438" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D438" s="2" t="s">
-        <v>697</v>
+        <v>715</v>
       </c>
       <c r="E438" s="2" t="s">
-        <v>708</v>
+        <v>726</v>
       </c>
       <c r="K438" s="2"/>
       <c r="L438" s="2"/>
@@ -10382,10 +10830,10 @@
         <v>6</v>
       </c>
       <c r="D439" s="2" t="s">
-        <v>698</v>
+        <v>716</v>
       </c>
       <c r="E439" s="2" t="s">
-        <v>709</v>
+        <v>727</v>
       </c>
       <c r="K439" s="2"/>
       <c r="L439" s="2"/>
@@ -10397,16 +10845,16 @@
         <v>439</v>
       </c>
       <c r="B440" t="s">
-        <v>699</v>
+        <v>717</v>
       </c>
       <c r="C440" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D440" s="2" t="s">
-        <v>700</v>
+        <v>718</v>
       </c>
       <c r="E440" s="2" t="s">
-        <v>710</v>
+        <v>728</v>
       </c>
       <c r="K440" s="2"/>
       <c r="L440" s="2"/>
@@ -10421,10 +10869,10 @@
         <v>6</v>
       </c>
       <c r="D441" s="2" t="s">
-        <v>701</v>
+        <v>719</v>
       </c>
       <c r="E441" s="2" t="s">
-        <v>711</v>
+        <v>729</v>
       </c>
       <c r="K441" s="2"/>
       <c r="L441" s="2"/>
@@ -10436,16 +10884,16 @@
         <v>441</v>
       </c>
       <c r="B442" t="s">
-        <v>712</v>
+        <v>730</v>
       </c>
       <c r="C442" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D442" s="2" t="s">
-        <v>713</v>
+        <v>731</v>
       </c>
       <c r="E442" s="2" t="s">
-        <v>727</v>
+        <v>745</v>
       </c>
       <c r="K442" s="2"/>
       <c r="L442" s="2"/>
@@ -10460,10 +10908,10 @@
         <v>6</v>
       </c>
       <c r="D443" s="2" t="s">
-        <v>714</v>
+        <v>732</v>
       </c>
       <c r="E443" s="2" t="s">
-        <v>728</v>
+        <v>746</v>
       </c>
       <c r="K443" s="2"/>
       <c r="L443" s="2"/>
@@ -10475,16 +10923,16 @@
         <v>443</v>
       </c>
       <c r="B444" t="s">
-        <v>715</v>
+        <v>733</v>
       </c>
       <c r="C444" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D444" s="2" t="s">
-        <v>716</v>
+        <v>734</v>
       </c>
       <c r="E444" s="2" t="s">
-        <v>729</v>
+        <v>747</v>
       </c>
       <c r="K444" s="2"/>
       <c r="L444" s="2"/>
@@ -10499,10 +10947,10 @@
         <v>6</v>
       </c>
       <c r="D445" s="2" t="s">
-        <v>717</v>
+        <v>735</v>
       </c>
       <c r="E445" s="2" t="s">
-        <v>730</v>
+        <v>748</v>
       </c>
       <c r="K445" s="2"/>
       <c r="L445" s="2"/>
@@ -10514,16 +10962,16 @@
         <v>445</v>
       </c>
       <c r="B446" t="s">
-        <v>718</v>
+        <v>736</v>
       </c>
       <c r="C446" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D446" s="2" t="s">
-        <v>719</v>
+        <v>737</v>
       </c>
       <c r="E446" s="2" t="s">
-        <v>731</v>
+        <v>749</v>
       </c>
       <c r="K446" s="2"/>
       <c r="L446" s="2"/>
@@ -10538,10 +10986,10 @@
         <v>6</v>
       </c>
       <c r="D447" s="2" t="s">
-        <v>720</v>
+        <v>738</v>
       </c>
       <c r="E447" s="2" t="s">
-        <v>732</v>
+        <v>750</v>
       </c>
       <c r="K447" s="2"/>
       <c r="L447" s="2"/>
@@ -10553,16 +11001,16 @@
         <v>447</v>
       </c>
       <c r="B448" t="s">
-        <v>721</v>
+        <v>739</v>
       </c>
       <c r="C448" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D448" s="2" t="s">
-        <v>722</v>
+        <v>740</v>
       </c>
       <c r="E448" s="2" t="s">
-        <v>733</v>
+        <v>751</v>
       </c>
       <c r="K448" s="2"/>
       <c r="L448" s="2"/>
@@ -10577,10 +11025,10 @@
         <v>6</v>
       </c>
       <c r="D449" s="2" t="s">
-        <v>723</v>
+        <v>741</v>
       </c>
       <c r="E449" s="2" t="s">
-        <v>734</v>
+        <v>752</v>
       </c>
       <c r="K449" s="2"/>
       <c r="L449" s="2"/>
@@ -10592,16 +11040,16 @@
         <v>449</v>
       </c>
       <c r="B450" t="s">
-        <v>724</v>
+        <v>742</v>
       </c>
       <c r="C450" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D450" s="2" t="s">
-        <v>725</v>
+        <v>743</v>
       </c>
       <c r="E450" s="2" t="s">
-        <v>735</v>
+        <v>753</v>
       </c>
       <c r="K450" s="2"/>
       <c r="L450" s="2"/>
@@ -10616,10 +11064,10 @@
         <v>6</v>
       </c>
       <c r="D451" s="2" t="s">
-        <v>726</v>
+        <v>744</v>
       </c>
       <c r="E451" s="2" t="s">
-        <v>736</v>
+        <v>754</v>
       </c>
       <c r="K451" s="2"/>
       <c r="L451" s="2"/>
@@ -10631,16 +11079,16 @@
         <v>451</v>
       </c>
       <c r="B452" t="s">
-        <v>737</v>
+        <v>755</v>
       </c>
       <c r="C452" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D452" s="2" t="s">
-        <v>738</v>
+        <v>756</v>
       </c>
       <c r="E452" s="2" t="s">
-        <v>752</v>
+        <v>770</v>
       </c>
       <c r="H452" s="5"/>
       <c r="I452" s="5"/>
@@ -10658,10 +11106,10 @@
         <v>6</v>
       </c>
       <c r="D453" s="2" t="s">
-        <v>739</v>
+        <v>757</v>
       </c>
       <c r="E453" s="2" t="s">
-        <v>753</v>
+        <v>771</v>
       </c>
       <c r="H453" s="2"/>
       <c r="I453" s="2"/>
@@ -10676,16 +11124,16 @@
         <v>453</v>
       </c>
       <c r="B454" t="s">
-        <v>742</v>
+        <v>760</v>
       </c>
       <c r="C454" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D454" s="2" t="s">
-        <v>740</v>
+        <v>758</v>
       </c>
       <c r="E454" s="2" t="s">
-        <v>754</v>
+        <v>772</v>
       </c>
       <c r="H454" s="2"/>
       <c r="I454" s="2"/>
@@ -10700,10 +11148,10 @@
         <v>6</v>
       </c>
       <c r="D455" s="2" t="s">
-        <v>741</v>
+        <v>759</v>
       </c>
       <c r="E455" s="2" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
       <c r="H455" s="2"/>
       <c r="I455" s="2"/>
@@ -10715,16 +11163,16 @@
         <v>455</v>
       </c>
       <c r="B456" t="s">
-        <v>743</v>
+        <v>761</v>
       </c>
       <c r="C456" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D456" s="2" t="s">
-        <v>744</v>
+        <v>762</v>
       </c>
       <c r="E456" s="2" t="s">
-        <v>756</v>
+        <v>774</v>
       </c>
       <c r="H456" s="2"/>
       <c r="I456" s="2"/>
@@ -10739,10 +11187,10 @@
         <v>6</v>
       </c>
       <c r="D457" s="2" t="s">
-        <v>745</v>
+        <v>763</v>
       </c>
       <c r="E457" s="2" t="s">
-        <v>757</v>
+        <v>775</v>
       </c>
       <c r="H457" s="2"/>
       <c r="I457" s="2"/>
@@ -10754,16 +11202,16 @@
         <v>457</v>
       </c>
       <c r="B458" t="s">
-        <v>746</v>
+        <v>764</v>
       </c>
       <c r="C458" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D458" s="2" t="s">
-        <v>747</v>
+        <v>765</v>
       </c>
       <c r="E458" s="2" t="s">
-        <v>758</v>
+        <v>776</v>
       </c>
       <c r="H458" s="2"/>
       <c r="I458" s="2"/>
@@ -10778,10 +11226,10 @@
         <v>6</v>
       </c>
       <c r="D459" s="2" t="s">
-        <v>748</v>
+        <v>766</v>
       </c>
       <c r="E459" s="2" t="s">
-        <v>759</v>
+        <v>777</v>
       </c>
       <c r="H459" s="2"/>
       <c r="I459" s="2"/>
@@ -10793,16 +11241,16 @@
         <v>459</v>
       </c>
       <c r="B460" t="s">
-        <v>749</v>
+        <v>767</v>
       </c>
       <c r="C460" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D460" s="2" t="s">
-        <v>750</v>
+        <v>768</v>
       </c>
       <c r="E460" s="2" t="s">
-        <v>760</v>
+        <v>778</v>
       </c>
       <c r="H460" s="2"/>
       <c r="I460" s="2"/>
@@ -10817,10 +11265,10 @@
         <v>6</v>
       </c>
       <c r="D461" s="2" t="s">
-        <v>751</v>
+        <v>769</v>
       </c>
       <c r="E461" s="2" t="s">
-        <v>761</v>
+        <v>779</v>
       </c>
       <c r="H461" s="2"/>
       <c r="I461" s="2"/>
@@ -10832,16 +11280,16 @@
         <v>461</v>
       </c>
       <c r="B462" t="s">
-        <v>762</v>
+        <v>780</v>
       </c>
       <c r="C462" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D462" s="2" t="s">
-        <v>763</v>
+        <v>781</v>
       </c>
       <c r="E462" s="2" t="s">
-        <v>765</v>
+        <v>783</v>
       </c>
       <c r="H462" s="2"/>
       <c r="I462" s="2"/>
@@ -10856,10 +11304,10 @@
         <v>6</v>
       </c>
       <c r="D463" s="2" t="s">
-        <v>764</v>
+        <v>782</v>
       </c>
       <c r="E463" s="2" t="s">
-        <v>766</v>
+        <v>784</v>
       </c>
     </row>
     <row r="464" spans="1:14" x14ac:dyDescent="0.3">
@@ -10867,16 +11315,16 @@
         <v>463</v>
       </c>
       <c r="B464" s="2" t="s">
-        <v>778</v>
+        <v>796</v>
       </c>
       <c r="C464" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D464" s="2" t="s">
-        <v>767</v>
+        <v>785</v>
       </c>
       <c r="E464" s="2" t="s">
-        <v>779</v>
+        <v>797</v>
       </c>
       <c r="J464" s="2"/>
       <c r="K464" s="2"/>
@@ -10891,10 +11339,10 @@
         <v>6</v>
       </c>
       <c r="D465" s="2" t="s">
-        <v>768</v>
+        <v>786</v>
       </c>
       <c r="E465" s="2" t="s">
-        <v>780</v>
+        <v>798</v>
       </c>
       <c r="J465" s="2"/>
       <c r="K465" s="2"/>
@@ -10906,16 +11354,16 @@
         <v>465</v>
       </c>
       <c r="B466" s="2" t="s">
-        <v>769</v>
+        <v>787</v>
       </c>
       <c r="C466" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D466" s="2" t="s">
-        <v>770</v>
+        <v>788</v>
       </c>
       <c r="E466" s="2" t="s">
-        <v>781</v>
+        <v>799</v>
       </c>
     </row>
     <row r="467" spans="1:13" x14ac:dyDescent="0.3">
@@ -10927,10 +11375,10 @@
         <v>6</v>
       </c>
       <c r="D467" s="2" t="s">
-        <v>771</v>
+        <v>789</v>
       </c>
       <c r="E467" s="2" t="s">
-        <v>782</v>
+        <v>800</v>
       </c>
     </row>
     <row r="468" spans="1:13" x14ac:dyDescent="0.3">
@@ -10938,16 +11386,16 @@
         <v>467</v>
       </c>
       <c r="B468" s="2" t="s">
-        <v>783</v>
+        <v>801</v>
       </c>
       <c r="C468" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D468" s="2" t="s">
-        <v>772</v>
+        <v>790</v>
       </c>
       <c r="E468" s="2" t="s">
-        <v>784</v>
+        <v>802</v>
       </c>
     </row>
     <row r="469" spans="1:13" x14ac:dyDescent="0.3">
@@ -10959,10 +11407,10 @@
         <v>6</v>
       </c>
       <c r="D469" s="2" t="s">
-        <v>773</v>
+        <v>791</v>
       </c>
       <c r="E469" s="2" t="s">
-        <v>785</v>
+        <v>803</v>
       </c>
     </row>
     <row r="470" spans="1:13" x14ac:dyDescent="0.3">
@@ -10970,16 +11418,16 @@
         <v>469</v>
       </c>
       <c r="B470" s="2" t="s">
-        <v>786</v>
+        <v>804</v>
       </c>
       <c r="C470" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D470" s="2" t="s">
-        <v>774</v>
+        <v>792</v>
       </c>
       <c r="E470" s="2" t="s">
-        <v>787</v>
+        <v>805</v>
       </c>
     </row>
     <row r="471" spans="1:13" x14ac:dyDescent="0.3">
@@ -10991,10 +11439,10 @@
         <v>6</v>
       </c>
       <c r="D471" s="2" t="s">
-        <v>775</v>
+        <v>793</v>
       </c>
       <c r="E471" s="2" t="s">
-        <v>788</v>
+        <v>806</v>
       </c>
     </row>
     <row r="472" spans="1:13" x14ac:dyDescent="0.3">
@@ -11002,16 +11450,16 @@
         <v>471</v>
       </c>
       <c r="B472" s="2" t="s">
-        <v>789</v>
+        <v>807</v>
       </c>
       <c r="C472" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D472" s="2" t="s">
-        <v>776</v>
+        <v>794</v>
       </c>
       <c r="E472" s="2" t="s">
-        <v>790</v>
+        <v>808</v>
       </c>
     </row>
     <row r="473" spans="1:13" x14ac:dyDescent="0.3">
@@ -11023,10 +11471,10 @@
         <v>6</v>
       </c>
       <c r="D473" s="2" t="s">
-        <v>777</v>
+        <v>795</v>
       </c>
       <c r="E473" s="2" t="s">
-        <v>791</v>
+        <v>809</v>
       </c>
     </row>
     <row r="474" spans="1:13" x14ac:dyDescent="0.3">
@@ -11034,16 +11482,16 @@
         <v>473</v>
       </c>
       <c r="B474" s="2" t="s">
-        <v>792</v>
+        <v>810</v>
       </c>
       <c r="C474" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D474" s="2" t="s">
-        <v>793</v>
+        <v>811</v>
       </c>
       <c r="E474" s="2" t="s">
-        <v>804</v>
+        <v>822</v>
       </c>
     </row>
     <row r="475" spans="1:13" x14ac:dyDescent="0.3">
@@ -11055,10 +11503,10 @@
         <v>6</v>
       </c>
       <c r="D475" s="2" t="s">
-        <v>794</v>
+        <v>812</v>
       </c>
       <c r="E475" s="2" t="s">
-        <v>805</v>
+        <v>823</v>
       </c>
     </row>
     <row r="476" spans="1:13" x14ac:dyDescent="0.3">
@@ -11066,16 +11514,16 @@
         <v>475</v>
       </c>
       <c r="B476" s="2" t="s">
-        <v>795</v>
+        <v>813</v>
       </c>
       <c r="C476" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D476" s="2" t="s">
-        <v>806</v>
+        <v>824</v>
       </c>
       <c r="E476" s="2" t="s">
-        <v>807</v>
+        <v>825</v>
       </c>
     </row>
     <row r="477" spans="1:13" x14ac:dyDescent="0.3">
@@ -11087,10 +11535,10 @@
         <v>6</v>
       </c>
       <c r="D477" s="2" t="s">
-        <v>808</v>
+        <v>826</v>
       </c>
       <c r="E477" s="2" t="s">
-        <v>809</v>
+        <v>827</v>
       </c>
     </row>
     <row r="478" spans="1:13" x14ac:dyDescent="0.3">
@@ -11098,16 +11546,16 @@
         <v>477</v>
       </c>
       <c r="B478" s="2" t="s">
-        <v>796</v>
+        <v>814</v>
       </c>
       <c r="C478" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D478" s="2" t="s">
-        <v>985</v>
+        <v>1003</v>
       </c>
       <c r="E478" s="2" t="s">
-        <v>810</v>
+        <v>828</v>
       </c>
     </row>
     <row r="479" spans="1:13" x14ac:dyDescent="0.3">
@@ -11119,10 +11567,10 @@
         <v>6</v>
       </c>
       <c r="D479" s="2" t="s">
-        <v>797</v>
+        <v>815</v>
       </c>
       <c r="E479" s="2" t="s">
-        <v>811</v>
+        <v>829</v>
       </c>
     </row>
     <row r="480" spans="1:13" x14ac:dyDescent="0.3">
@@ -11130,16 +11578,16 @@
         <v>479</v>
       </c>
       <c r="B480" s="2" t="s">
-        <v>798</v>
+        <v>816</v>
       </c>
       <c r="C480" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D480" s="2" t="s">
-        <v>799</v>
+        <v>817</v>
       </c>
       <c r="E480" s="2" t="s">
-        <v>812</v>
+        <v>830</v>
       </c>
     </row>
     <row r="481" spans="1:5" x14ac:dyDescent="0.3">
@@ -11151,10 +11599,10 @@
         <v>6</v>
       </c>
       <c r="D481" s="2" t="s">
-        <v>800</v>
+        <v>818</v>
       </c>
       <c r="E481" s="2" t="s">
-        <v>813</v>
+        <v>831</v>
       </c>
     </row>
     <row r="482" spans="1:5" x14ac:dyDescent="0.3">
@@ -11162,16 +11610,16 @@
         <v>481</v>
       </c>
       <c r="B482" s="2" t="s">
-        <v>801</v>
+        <v>819</v>
       </c>
       <c r="C482" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D482" s="2" t="s">
-        <v>802</v>
+        <v>820</v>
       </c>
       <c r="E482" s="2" t="s">
-        <v>814</v>
+        <v>832</v>
       </c>
     </row>
     <row r="483" spans="1:5" x14ac:dyDescent="0.3">
@@ -11183,10 +11631,10 @@
         <v>6</v>
       </c>
       <c r="D483" s="2" t="s">
-        <v>803</v>
+        <v>821</v>
       </c>
       <c r="E483" s="2" t="s">
-        <v>815</v>
+        <v>833</v>
       </c>
     </row>
     <row r="484" spans="1:5" x14ac:dyDescent="0.3">
@@ -11194,16 +11642,16 @@
         <v>483</v>
       </c>
       <c r="B484" s="2" t="s">
-        <v>816</v>
+        <v>834</v>
       </c>
       <c r="C484" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D484" s="2" t="s">
-        <v>817</v>
+        <v>835</v>
       </c>
       <c r="E484" s="2" t="s">
-        <v>826</v>
+        <v>844</v>
       </c>
     </row>
     <row r="485" spans="1:5" x14ac:dyDescent="0.3">
@@ -11215,10 +11663,10 @@
         <v>6</v>
       </c>
       <c r="D485" s="2" t="s">
-        <v>818</v>
+        <v>836</v>
       </c>
       <c r="E485" s="2" t="s">
-        <v>827</v>
+        <v>845</v>
       </c>
     </row>
     <row r="486" spans="1:5" x14ac:dyDescent="0.3">
@@ -11226,16 +11674,16 @@
         <v>485</v>
       </c>
       <c r="B486" s="2" t="s">
-        <v>819</v>
+        <v>837</v>
       </c>
       <c r="C486" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D486" s="2" t="s">
-        <v>820</v>
+        <v>838</v>
       </c>
       <c r="E486" s="2" t="s">
-        <v>828</v>
+        <v>846</v>
       </c>
     </row>
     <row r="487" spans="1:5" x14ac:dyDescent="0.3">
@@ -11247,10 +11695,10 @@
         <v>6</v>
       </c>
       <c r="D487" s="2" t="s">
-        <v>821</v>
+        <v>839</v>
       </c>
       <c r="E487" s="2" t="s">
-        <v>829</v>
+        <v>847</v>
       </c>
     </row>
     <row r="488" spans="1:5" x14ac:dyDescent="0.3">
@@ -11258,16 +11706,16 @@
         <v>487</v>
       </c>
       <c r="B488" s="2" t="s">
-        <v>822</v>
+        <v>840</v>
       </c>
       <c r="C488" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D488" s="2" t="s">
-        <v>986</v>
+        <v>1004</v>
       </c>
       <c r="E488" s="2" t="s">
-        <v>830</v>
+        <v>848</v>
       </c>
     </row>
     <row r="489" spans="1:5" x14ac:dyDescent="0.3">
@@ -11279,10 +11727,10 @@
         <v>6</v>
       </c>
       <c r="D489" s="2" t="s">
-        <v>987</v>
+        <v>1005</v>
       </c>
       <c r="E489" s="2" t="s">
-        <v>831</v>
+        <v>849</v>
       </c>
     </row>
     <row r="490" spans="1:5" x14ac:dyDescent="0.3">
@@ -11290,16 +11738,16 @@
         <v>489</v>
       </c>
       <c r="B490" s="2" t="s">
-        <v>823</v>
+        <v>841</v>
       </c>
       <c r="C490" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D490" s="2" t="s">
-        <v>832</v>
+        <v>850</v>
       </c>
       <c r="E490" s="2" t="s">
-        <v>833</v>
+        <v>851</v>
       </c>
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.3">
@@ -11311,10 +11759,10 @@
         <v>6</v>
       </c>
       <c r="D491" s="2" t="s">
-        <v>834</v>
+        <v>852</v>
       </c>
       <c r="E491" s="2" t="s">
-        <v>835</v>
+        <v>853</v>
       </c>
     </row>
     <row r="492" spans="1:5" x14ac:dyDescent="0.3">
@@ -11322,16 +11770,16 @@
         <v>491</v>
       </c>
       <c r="B492" s="2" t="s">
-        <v>838</v>
+        <v>856</v>
       </c>
       <c r="C492" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D492" s="2" t="s">
-        <v>824</v>
+        <v>842</v>
       </c>
       <c r="E492" s="2" t="s">
-        <v>836</v>
+        <v>854</v>
       </c>
     </row>
     <row r="493" spans="1:5" x14ac:dyDescent="0.3">
@@ -11343,10 +11791,10 @@
         <v>6</v>
       </c>
       <c r="D493" s="2" t="s">
-        <v>825</v>
+        <v>843</v>
       </c>
       <c r="E493" s="2" t="s">
-        <v>837</v>
+        <v>855</v>
       </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.3">
@@ -11354,16 +11802,16 @@
         <v>493</v>
       </c>
       <c r="B494" s="2" t="s">
-        <v>849</v>
+        <v>867</v>
       </c>
       <c r="C494" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D494" s="2" t="s">
-        <v>839</v>
+        <v>857</v>
       </c>
       <c r="E494" s="2" t="s">
-        <v>850</v>
+        <v>868</v>
       </c>
     </row>
     <row r="495" spans="1:5" x14ac:dyDescent="0.3">
@@ -11375,10 +11823,10 @@
         <v>6</v>
       </c>
       <c r="D495" s="2" t="s">
-        <v>840</v>
+        <v>858</v>
       </c>
       <c r="E495" s="2" t="s">
-        <v>851</v>
+        <v>869</v>
       </c>
     </row>
     <row r="496" spans="1:5" x14ac:dyDescent="0.3">
@@ -11386,16 +11834,16 @@
         <v>495</v>
       </c>
       <c r="B496" s="2" t="s">
-        <v>852</v>
+        <v>870</v>
       </c>
       <c r="C496" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D496" s="2" t="s">
-        <v>841</v>
+        <v>859</v>
       </c>
       <c r="E496" s="2" t="s">
-        <v>853</v>
+        <v>871</v>
       </c>
     </row>
     <row r="497" spans="1:5" x14ac:dyDescent="0.3">
@@ -11407,10 +11855,10 @@
         <v>6</v>
       </c>
       <c r="D497" s="2" t="s">
-        <v>842</v>
+        <v>860</v>
       </c>
       <c r="E497" s="2" t="s">
-        <v>854</v>
+        <v>872</v>
       </c>
     </row>
     <row r="498" spans="1:5" x14ac:dyDescent="0.3">
@@ -11418,16 +11866,16 @@
         <v>497</v>
       </c>
       <c r="B498" s="2" t="s">
-        <v>855</v>
+        <v>873</v>
       </c>
       <c r="C498" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D498" s="2" t="s">
-        <v>843</v>
+        <v>861</v>
       </c>
       <c r="E498" s="2" t="s">
-        <v>856</v>
+        <v>874</v>
       </c>
     </row>
     <row r="499" spans="1:5" x14ac:dyDescent="0.3">
@@ -11439,10 +11887,10 @@
         <v>6</v>
       </c>
       <c r="D499" s="2" t="s">
-        <v>844</v>
+        <v>862</v>
       </c>
       <c r="E499" s="2" t="s">
-        <v>857</v>
+        <v>875</v>
       </c>
     </row>
     <row r="500" spans="1:5" x14ac:dyDescent="0.3">
@@ -11450,16 +11898,16 @@
         <v>499</v>
       </c>
       <c r="B500" s="2" t="s">
-        <v>858</v>
+        <v>876</v>
       </c>
       <c r="C500" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D500" s="2" t="s">
-        <v>845</v>
+        <v>863</v>
       </c>
       <c r="E500" s="2" t="s">
-        <v>859</v>
+        <v>877</v>
       </c>
     </row>
     <row r="501" spans="1:5" x14ac:dyDescent="0.3">
@@ -11471,10 +11919,10 @@
         <v>6</v>
       </c>
       <c r="D501" s="2" t="s">
-        <v>846</v>
+        <v>864</v>
       </c>
       <c r="E501" s="2" t="s">
-        <v>860</v>
+        <v>878</v>
       </c>
     </row>
     <row r="502" spans="1:5" x14ac:dyDescent="0.3">
@@ -11482,16 +11930,16 @@
         <v>501</v>
       </c>
       <c r="B502" s="2" t="s">
-        <v>863</v>
+        <v>881</v>
       </c>
       <c r="C502" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D502" s="2" t="s">
-        <v>847</v>
+        <v>865</v>
       </c>
       <c r="E502" s="2" t="s">
-        <v>861</v>
+        <v>879</v>
       </c>
     </row>
     <row r="503" spans="1:5" x14ac:dyDescent="0.3">
@@ -11503,10 +11951,10 @@
         <v>6</v>
       </c>
       <c r="D503" s="2" t="s">
-        <v>848</v>
+        <v>866</v>
       </c>
       <c r="E503" s="2" t="s">
-        <v>862</v>
+        <v>880</v>
       </c>
     </row>
     <row r="504" spans="1:5" x14ac:dyDescent="0.3">
@@ -11514,16 +11962,16 @@
         <v>503</v>
       </c>
       <c r="B504" s="2" t="s">
-        <v>868</v>
+        <v>886</v>
       </c>
       <c r="C504" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D504" s="2" t="s">
-        <v>869</v>
+        <v>887</v>
       </c>
       <c r="E504" s="2" t="s">
-        <v>870</v>
+        <v>888</v>
       </c>
     </row>
     <row r="505" spans="1:5" x14ac:dyDescent="0.3">
@@ -11535,10 +11983,10 @@
         <v>6</v>
       </c>
       <c r="D505" s="2" t="s">
-        <v>871</v>
+        <v>889</v>
       </c>
       <c r="E505" s="2" t="s">
-        <v>872</v>
+        <v>890</v>
       </c>
     </row>
     <row r="506" spans="1:5" x14ac:dyDescent="0.3">
@@ -11546,16 +11994,16 @@
         <v>505</v>
       </c>
       <c r="B506" s="2" t="s">
-        <v>873</v>
+        <v>891</v>
       </c>
       <c r="C506" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D506" s="2" t="s">
-        <v>874</v>
+        <v>892</v>
       </c>
       <c r="E506" s="2" t="s">
-        <v>875</v>
+        <v>893</v>
       </c>
     </row>
     <row r="507" spans="1:5" x14ac:dyDescent="0.3">
@@ -11567,10 +12015,10 @@
         <v>6</v>
       </c>
       <c r="D507" s="2" t="s">
-        <v>876</v>
+        <v>894</v>
       </c>
       <c r="E507" s="2" t="s">
-        <v>877</v>
+        <v>895</v>
       </c>
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.3">
@@ -11578,16 +12026,16 @@
         <v>507</v>
       </c>
       <c r="B508" s="2" t="s">
-        <v>878</v>
+        <v>896</v>
       </c>
       <c r="C508" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D508" s="2" t="s">
-        <v>864</v>
+        <v>882</v>
       </c>
       <c r="E508" s="2" t="s">
-        <v>879</v>
+        <v>897</v>
       </c>
     </row>
     <row r="509" spans="1:5" x14ac:dyDescent="0.3">
@@ -11599,10 +12047,10 @@
         <v>6</v>
       </c>
       <c r="D509" s="2" t="s">
-        <v>865</v>
+        <v>883</v>
       </c>
       <c r="E509" s="2" t="s">
-        <v>880</v>
+        <v>898</v>
       </c>
     </row>
     <row r="510" spans="1:5" x14ac:dyDescent="0.3">
@@ -11610,16 +12058,16 @@
         <v>509</v>
       </c>
       <c r="B510" s="2" t="s">
-        <v>881</v>
+        <v>899</v>
       </c>
       <c r="C510" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D510" s="2" t="s">
-        <v>866</v>
+        <v>884</v>
       </c>
       <c r="E510" s="2" t="s">
-        <v>882</v>
+        <v>900</v>
       </c>
     </row>
     <row r="511" spans="1:5" x14ac:dyDescent="0.3">
@@ -11631,10 +12079,10 @@
         <v>6</v>
       </c>
       <c r="D511" s="2" t="s">
-        <v>883</v>
+        <v>901</v>
       </c>
       <c r="E511" s="2" t="s">
-        <v>884</v>
+        <v>902</v>
       </c>
     </row>
     <row r="512" spans="1:5" x14ac:dyDescent="0.3">
@@ -11642,16 +12090,16 @@
         <v>511</v>
       </c>
       <c r="B512" s="2" t="s">
-        <v>885</v>
+        <v>903</v>
       </c>
       <c r="C512" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D512" s="2" t="s">
-        <v>886</v>
+        <v>904</v>
       </c>
       <c r="E512" s="2" t="s">
-        <v>887</v>
+        <v>905</v>
       </c>
     </row>
     <row r="513" spans="1:5" x14ac:dyDescent="0.3">
@@ -11663,10 +12111,10 @@
         <v>6</v>
       </c>
       <c r="D513" s="2" t="s">
-        <v>867</v>
+        <v>885</v>
       </c>
       <c r="E513" s="2" t="s">
-        <v>888</v>
+        <v>906</v>
       </c>
     </row>
     <row r="514" spans="1:5" x14ac:dyDescent="0.3">
@@ -11674,16 +12122,16 @@
         <v>513</v>
       </c>
       <c r="B514" s="2" t="s">
-        <v>900</v>
+        <v>918</v>
       </c>
       <c r="C514" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D514" s="2" t="s">
-        <v>889</v>
+        <v>907</v>
       </c>
       <c r="E514" s="2" t="s">
-        <v>901</v>
+        <v>919</v>
       </c>
     </row>
     <row r="515" spans="1:5" x14ac:dyDescent="0.3">
@@ -11695,10 +12143,10 @@
         <v>6</v>
       </c>
       <c r="D515" s="2" t="s">
-        <v>890</v>
+        <v>908</v>
       </c>
       <c r="E515" s="2" t="s">
-        <v>902</v>
+        <v>920</v>
       </c>
     </row>
     <row r="516" spans="1:5" x14ac:dyDescent="0.3">
@@ -11706,16 +12154,16 @@
         <v>515</v>
       </c>
       <c r="B516" s="2" t="s">
-        <v>891</v>
+        <v>909</v>
       </c>
       <c r="C516" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D516" s="2" t="s">
-        <v>912</v>
+        <v>930</v>
       </c>
       <c r="E516" s="2" t="s">
-        <v>903</v>
+        <v>921</v>
       </c>
     </row>
     <row r="517" spans="1:5" x14ac:dyDescent="0.3">
@@ -11727,10 +12175,10 @@
         <v>6</v>
       </c>
       <c r="D517" s="2" t="s">
-        <v>913</v>
+        <v>931</v>
       </c>
       <c r="E517" s="2" t="s">
-        <v>904</v>
+        <v>922</v>
       </c>
     </row>
     <row r="518" spans="1:5" x14ac:dyDescent="0.3">
@@ -11738,16 +12186,16 @@
         <v>517</v>
       </c>
       <c r="B518" s="2" t="s">
-        <v>905</v>
+        <v>923</v>
       </c>
       <c r="C518" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D518" s="2" t="s">
-        <v>892</v>
+        <v>910</v>
       </c>
       <c r="E518" s="2" t="s">
-        <v>906</v>
+        <v>924</v>
       </c>
     </row>
     <row r="519" spans="1:5" x14ac:dyDescent="0.3">
@@ -11759,10 +12207,10 @@
         <v>6</v>
       </c>
       <c r="D519" s="2" t="s">
-        <v>893</v>
+        <v>911</v>
       </c>
       <c r="E519" s="2" t="s">
-        <v>907</v>
+        <v>925</v>
       </c>
     </row>
     <row r="520" spans="1:5" x14ac:dyDescent="0.3">
@@ -11770,16 +12218,16 @@
         <v>519</v>
       </c>
       <c r="B520" s="2" t="s">
-        <v>894</v>
+        <v>912</v>
       </c>
       <c r="C520" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D520" s="2" t="s">
-        <v>895</v>
+        <v>913</v>
       </c>
       <c r="E520" s="2" t="s">
-        <v>908</v>
+        <v>926</v>
       </c>
     </row>
     <row r="521" spans="1:5" x14ac:dyDescent="0.3">
@@ -11791,10 +12239,10 @@
         <v>6</v>
       </c>
       <c r="D521" s="2" t="s">
-        <v>896</v>
+        <v>914</v>
       </c>
       <c r="E521" s="2" t="s">
-        <v>909</v>
+        <v>927</v>
       </c>
     </row>
     <row r="522" spans="1:5" x14ac:dyDescent="0.3">
@@ -11802,16 +12250,16 @@
         <v>521</v>
       </c>
       <c r="B522" s="2" t="s">
-        <v>897</v>
+        <v>915</v>
       </c>
       <c r="C522" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D522" s="2" t="s">
-        <v>898</v>
+        <v>916</v>
       </c>
       <c r="E522" s="2" t="s">
-        <v>910</v>
+        <v>928</v>
       </c>
     </row>
     <row r="523" spans="1:5" x14ac:dyDescent="0.3">
@@ -11823,10 +12271,10 @@
         <v>6</v>
       </c>
       <c r="D523" s="2" t="s">
-        <v>899</v>
+        <v>917</v>
       </c>
       <c r="E523" s="2" t="s">
-        <v>911</v>
+        <v>929</v>
       </c>
     </row>
     <row r="524" spans="1:5" x14ac:dyDescent="0.3">
@@ -11834,16 +12282,16 @@
         <v>523</v>
       </c>
       <c r="B524" s="2" t="s">
-        <v>927</v>
+        <v>945</v>
       </c>
       <c r="C524" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D524" s="2" t="s">
-        <v>915</v>
+        <v>933</v>
       </c>
       <c r="E524" s="2" t="s">
-        <v>928</v>
+        <v>946</v>
       </c>
     </row>
     <row r="525" spans="1:5" x14ac:dyDescent="0.3">
@@ -11855,10 +12303,10 @@
         <v>6</v>
       </c>
       <c r="D525" s="2" t="s">
-        <v>914</v>
+        <v>932</v>
       </c>
       <c r="E525" s="2" t="s">
-        <v>929</v>
+        <v>947</v>
       </c>
     </row>
     <row r="526" spans="1:5" x14ac:dyDescent="0.3">
@@ -11866,16 +12314,16 @@
         <v>525</v>
       </c>
       <c r="B526" s="2" t="s">
-        <v>918</v>
+        <v>936</v>
       </c>
       <c r="C526" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D526" s="2" t="s">
-        <v>916</v>
+        <v>934</v>
       </c>
       <c r="E526" s="2" t="s">
-        <v>930</v>
+        <v>948</v>
       </c>
     </row>
     <row r="527" spans="1:5" x14ac:dyDescent="0.3">
@@ -11887,10 +12335,10 @@
         <v>6</v>
       </c>
       <c r="D527" s="2" t="s">
-        <v>917</v>
+        <v>935</v>
       </c>
       <c r="E527" s="2" t="s">
-        <v>931</v>
+        <v>949</v>
       </c>
     </row>
     <row r="528" spans="1:5" x14ac:dyDescent="0.3">
@@ -11898,16 +12346,16 @@
         <v>527</v>
       </c>
       <c r="B528" s="2" t="s">
-        <v>919</v>
+        <v>937</v>
       </c>
       <c r="C528" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D528" s="2" t="s">
-        <v>920</v>
+        <v>938</v>
       </c>
       <c r="E528" s="2" t="s">
-        <v>932</v>
+        <v>950</v>
       </c>
     </row>
     <row r="529" spans="1:5" x14ac:dyDescent="0.3">
@@ -11919,10 +12367,10 @@
         <v>6</v>
       </c>
       <c r="D529" s="2" t="s">
-        <v>921</v>
+        <v>939</v>
       </c>
       <c r="E529" s="2" t="s">
-        <v>933</v>
+        <v>951</v>
       </c>
     </row>
     <row r="530" spans="1:5" x14ac:dyDescent="0.3">
@@ -11930,16 +12378,16 @@
         <v>529</v>
       </c>
       <c r="B530" s="2" t="s">
-        <v>922</v>
+        <v>940</v>
       </c>
       <c r="C530" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D530" s="2" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
       <c r="E530" s="2" t="s">
-        <v>934</v>
+        <v>952</v>
       </c>
     </row>
     <row r="531" spans="1:5" x14ac:dyDescent="0.3">
@@ -11951,10 +12399,10 @@
         <v>6</v>
       </c>
       <c r="D531" s="2" t="s">
-        <v>924</v>
+        <v>942</v>
       </c>
       <c r="E531" s="2" t="s">
-        <v>935</v>
+        <v>953</v>
       </c>
     </row>
     <row r="532" spans="1:5" x14ac:dyDescent="0.3">
@@ -11962,16 +12410,16 @@
         <v>531</v>
       </c>
       <c r="B532" s="2" t="s">
-        <v>936</v>
+        <v>954</v>
       </c>
       <c r="C532" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D532" s="2" t="s">
-        <v>926</v>
+        <v>944</v>
       </c>
       <c r="E532" s="2" t="s">
-        <v>937</v>
+        <v>955</v>
       </c>
     </row>
     <row r="533" spans="1:5" x14ac:dyDescent="0.3">
@@ -11983,10 +12431,10 @@
         <v>6</v>
       </c>
       <c r="D533" s="2" t="s">
-        <v>925</v>
+        <v>943</v>
       </c>
       <c r="E533" s="2" t="s">
-        <v>938</v>
+        <v>956</v>
       </c>
     </row>
     <row r="534" spans="1:5" x14ac:dyDescent="0.3">
@@ -11994,16 +12442,16 @@
         <v>533</v>
       </c>
       <c r="B534" s="2" t="s">
-        <v>939</v>
+        <v>957</v>
       </c>
       <c r="C534" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D534" s="2" t="s">
-        <v>940</v>
+        <v>958</v>
       </c>
       <c r="E534" s="2" t="s">
-        <v>956</v>
+        <v>974</v>
       </c>
     </row>
     <row r="535" spans="1:5" x14ac:dyDescent="0.3">
@@ -12015,10 +12463,10 @@
         <v>6</v>
       </c>
       <c r="D535" s="2" t="s">
-        <v>941</v>
+        <v>959</v>
       </c>
       <c r="E535" s="2" t="s">
-        <v>957</v>
+        <v>975</v>
       </c>
     </row>
     <row r="536" spans="1:5" x14ac:dyDescent="0.3">
@@ -12026,16 +12474,16 @@
         <v>535</v>
       </c>
       <c r="B536" s="2" t="s">
-        <v>976</v>
+        <v>994</v>
       </c>
       <c r="C536" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D536" s="2" t="s">
-        <v>942</v>
+        <v>960</v>
       </c>
       <c r="E536" s="2" t="s">
-        <v>958</v>
+        <v>976</v>
       </c>
     </row>
     <row r="537" spans="1:5" x14ac:dyDescent="0.3">
@@ -12047,10 +12495,10 @@
         <v>6</v>
       </c>
       <c r="D537" s="2" t="s">
-        <v>943</v>
+        <v>961</v>
       </c>
       <c r="E537" s="2" t="s">
-        <v>959</v>
+        <v>977</v>
       </c>
     </row>
     <row r="538" spans="1:5" x14ac:dyDescent="0.3">
@@ -12058,16 +12506,16 @@
         <v>537</v>
       </c>
       <c r="B538" s="2" t="s">
-        <v>944</v>
+        <v>962</v>
       </c>
       <c r="C538" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D538" s="2" t="s">
-        <v>945</v>
+        <v>963</v>
       </c>
       <c r="E538" s="2" t="s">
-        <v>960</v>
+        <v>978</v>
       </c>
     </row>
     <row r="539" spans="1:5" x14ac:dyDescent="0.3">
@@ -12079,10 +12527,10 @@
         <v>6</v>
       </c>
       <c r="D539" s="2" t="s">
-        <v>946</v>
+        <v>964</v>
       </c>
       <c r="E539" s="2" t="s">
-        <v>961</v>
+        <v>979</v>
       </c>
     </row>
     <row r="540" spans="1:5" x14ac:dyDescent="0.3">
@@ -12090,16 +12538,16 @@
         <v>539</v>
       </c>
       <c r="B540" s="2" t="s">
-        <v>977</v>
+        <v>995</v>
       </c>
       <c r="C540" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D540" s="2" t="s">
-        <v>947</v>
+        <v>965</v>
       </c>
       <c r="E540" s="2" t="s">
-        <v>962</v>
+        <v>980</v>
       </c>
     </row>
     <row r="541" spans="1:5" x14ac:dyDescent="0.3">
@@ -12111,10 +12559,10 @@
         <v>6</v>
       </c>
       <c r="D541" s="2" t="s">
-        <v>948</v>
+        <v>966</v>
       </c>
       <c r="E541" s="2" t="s">
-        <v>963</v>
+        <v>981</v>
       </c>
     </row>
     <row r="542" spans="1:5" x14ac:dyDescent="0.3">
@@ -12122,16 +12570,16 @@
         <v>541</v>
       </c>
       <c r="B542" s="2" t="s">
-        <v>978</v>
+        <v>996</v>
       </c>
       <c r="C542" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D542" s="2" t="s">
-        <v>949</v>
+        <v>967</v>
       </c>
       <c r="E542" s="2" t="s">
-        <v>964</v>
+        <v>982</v>
       </c>
     </row>
     <row r="543" spans="1:5" x14ac:dyDescent="0.3">
@@ -12143,10 +12591,10 @@
         <v>6</v>
       </c>
       <c r="D543" s="2" t="s">
-        <v>950</v>
+        <v>968</v>
       </c>
       <c r="E543" s="2" t="s">
-        <v>965</v>
+        <v>983</v>
       </c>
     </row>
     <row r="544" spans="1:5" x14ac:dyDescent="0.3">
@@ -12154,16 +12602,16 @@
         <v>543</v>
       </c>
       <c r="B544" s="2" t="s">
-        <v>979</v>
+        <v>997</v>
       </c>
       <c r="C544" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D544" s="2" t="s">
-        <v>990</v>
+        <v>1008</v>
       </c>
       <c r="E544" s="2" t="s">
-        <v>966</v>
+        <v>984</v>
       </c>
     </row>
     <row r="545" spans="1:5" x14ac:dyDescent="0.3">
@@ -12175,10 +12623,10 @@
         <v>6</v>
       </c>
       <c r="D545" s="2" t="s">
-        <v>952</v>
+        <v>970</v>
       </c>
       <c r="E545" s="2" t="s">
-        <v>967</v>
+        <v>985</v>
       </c>
     </row>
     <row r="546" spans="1:5" x14ac:dyDescent="0.3">
@@ -12186,16 +12634,16 @@
         <v>545</v>
       </c>
       <c r="B546" s="2" t="s">
-        <v>980</v>
+        <v>998</v>
       </c>
       <c r="C546" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D546" s="2" t="s">
-        <v>989</v>
+        <v>1007</v>
       </c>
       <c r="E546" s="2" t="s">
-        <v>968</v>
+        <v>986</v>
       </c>
     </row>
     <row r="547" spans="1:5" x14ac:dyDescent="0.3">
@@ -12207,10 +12655,10 @@
         <v>6</v>
       </c>
       <c r="D547" s="2" t="s">
-        <v>951</v>
+        <v>969</v>
       </c>
       <c r="E547" s="2" t="s">
-        <v>969</v>
+        <v>987</v>
       </c>
     </row>
     <row r="548" spans="1:5" x14ac:dyDescent="0.3">
@@ -12218,16 +12666,16 @@
         <v>547</v>
       </c>
       <c r="B548" s="2" t="s">
-        <v>981</v>
+        <v>999</v>
       </c>
       <c r="C548" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D548" s="2" t="s">
-        <v>991</v>
+        <v>1009</v>
       </c>
       <c r="E548" s="2" t="s">
-        <v>970</v>
+        <v>988</v>
       </c>
     </row>
     <row r="549" spans="1:5" x14ac:dyDescent="0.3">
@@ -12239,10 +12687,10 @@
         <v>6</v>
       </c>
       <c r="D549" s="2" t="s">
-        <v>988</v>
+        <v>1006</v>
       </c>
       <c r="E549" s="2" t="s">
-        <v>971</v>
+        <v>989</v>
       </c>
     </row>
     <row r="550" spans="1:5" x14ac:dyDescent="0.3">
@@ -12250,16 +12698,16 @@
         <v>549</v>
       </c>
       <c r="B550" s="2" t="s">
-        <v>982</v>
+        <v>1000</v>
       </c>
       <c r="C550" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D550" s="2" t="s">
-        <v>983</v>
+        <v>1001</v>
       </c>
       <c r="E550" s="2" t="s">
-        <v>972</v>
+        <v>990</v>
       </c>
     </row>
     <row r="551" spans="1:5" x14ac:dyDescent="0.3">
@@ -12271,10 +12719,10 @@
         <v>6</v>
       </c>
       <c r="D551" s="2" t="s">
-        <v>984</v>
+        <v>1002</v>
       </c>
       <c r="E551" s="2" t="s">
-        <v>973</v>
+        <v>991</v>
       </c>
     </row>
     <row r="552" spans="1:5" x14ac:dyDescent="0.3">
@@ -12282,16 +12730,16 @@
         <v>551</v>
       </c>
       <c r="B552" s="2" t="s">
-        <v>953</v>
+        <v>971</v>
       </c>
       <c r="C552" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D552" s="2" t="s">
-        <v>954</v>
+        <v>972</v>
       </c>
       <c r="E552" s="2" t="s">
-        <v>974</v>
+        <v>992</v>
       </c>
     </row>
     <row r="553" spans="1:5" x14ac:dyDescent="0.3">
@@ -12303,10 +12751,10 @@
         <v>6</v>
       </c>
       <c r="D553" s="2" t="s">
-        <v>955</v>
+        <v>973</v>
       </c>
       <c r="E553" s="2" t="s">
-        <v>975</v>
+        <v>993</v>
       </c>
     </row>
     <row r="554" spans="1:5" x14ac:dyDescent="0.3">
@@ -12653,8 +13101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53633261-343C-43E5-B2B3-7E483D444F25}">
   <dimension ref="E5:L435"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="J104" sqref="J104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -12684,13 +13132,13 @@
         <v>1</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>683</v>
+        <v>694</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>993</v>
+        <v>1011</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>684</v>
+        <v>695</v>
       </c>
     </row>
     <row r="7" spans="5:8" x14ac:dyDescent="0.3">
@@ -12698,13 +13146,13 @@
         <v>2</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>681</v>
+        <v>692</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>994</v>
+        <v>1012</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>682</v>
+        <v>693</v>
       </c>
     </row>
     <row r="8" spans="5:8" x14ac:dyDescent="0.3">
@@ -12712,13 +13160,13 @@
         <v>3</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>995</v>
+        <v>1013</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>1050</v>
+        <v>1068</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>1013</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="9" spans="5:8" x14ac:dyDescent="0.3">
@@ -12726,13 +13174,13 @@
         <v>4</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>685</v>
+        <v>696</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>996</v>
+        <v>1014</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>686</v>
+        <v>697</v>
       </c>
     </row>
     <row r="10" spans="5:8" x14ac:dyDescent="0.3">
@@ -12740,13 +13188,13 @@
         <v>5</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>997</v>
+        <v>1015</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>998</v>
+        <v>1016</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>1014</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="11" spans="5:8" x14ac:dyDescent="0.3">
@@ -12754,13 +13202,13 @@
         <v>6</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>999</v>
+        <v>1017</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>1000</v>
+        <v>1018</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>1015</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="12" spans="5:8" x14ac:dyDescent="0.3">
@@ -12768,13 +13216,13 @@
         <v>7</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>1001</v>
+        <v>1019</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>1002</v>
+        <v>1020</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>1016</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="13" spans="5:8" x14ac:dyDescent="0.3">
@@ -12782,27 +13230,27 @@
         <v>8</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>1003</v>
+        <v>1021</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>1004</v>
+        <v>1022</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>1017</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="14" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E14" s="4">
         <v>9</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>1160</v>
+      <c r="F14" s="6" t="s">
+        <v>1176</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>1005</v>
+        <v>1023</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>1018</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="15" spans="5:8" x14ac:dyDescent="0.3">
@@ -12813,10 +13261,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>1006</v>
+        <v>1024</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>1019</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="16" spans="5:8" x14ac:dyDescent="0.3">
@@ -12827,10 +13275,10 @@
         <v>2</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>1007</v>
+        <v>1025</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>1020</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.3">
@@ -12841,10 +13289,10 @@
         <v>3</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>1008</v>
+        <v>1026</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>1021</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.3">
@@ -12855,10 +13303,10 @@
         <v>4</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>1009</v>
+        <v>1027</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>1022</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="19" spans="5:12" x14ac:dyDescent="0.3">
@@ -12869,10 +13317,10 @@
         <v>5</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>1010</v>
+        <v>1028</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>1023</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="20" spans="5:12" x14ac:dyDescent="0.3">
@@ -12883,10 +13331,10 @@
         <v>6</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>1024</v>
+        <v>1042</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>1025</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="21" spans="5:12" x14ac:dyDescent="0.3">
@@ -12897,10 +13345,10 @@
         <v>7</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>1026</v>
+        <v>1044</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>1027</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="22" spans="5:12" x14ac:dyDescent="0.3">
@@ -12911,10 +13359,10 @@
         <v>8</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>1028</v>
+        <v>1046</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>1029</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="23" spans="5:12" x14ac:dyDescent="0.3">
@@ -12925,10 +13373,10 @@
         <v>9</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>1011</v>
+        <v>1029</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>1030</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="24" spans="5:12" x14ac:dyDescent="0.3">
@@ -12939,10 +13387,10 @@
         <v>10</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>1031</v>
+        <v>1049</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>1032</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="25" spans="5:12" x14ac:dyDescent="0.3">
@@ -12953,10 +13401,10 @@
         <v>677</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>1012</v>
+        <v>1030</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>1033</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="26" spans="5:12" x14ac:dyDescent="0.3">
@@ -12967,10 +13415,10 @@
         <v>678</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>1071</v>
+        <v>1089</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>1072</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="27" spans="5:12" x14ac:dyDescent="0.3">
@@ -12981,10 +13429,10 @@
         <v>679</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>1034</v>
+        <v>1052</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>1073</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="28" spans="5:12" x14ac:dyDescent="0.3">
@@ -12992,13 +13440,13 @@
         <v>23</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>1043</v>
+        <v>1061</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>1035</v>
+        <v>1053</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>1074</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="29" spans="5:12" x14ac:dyDescent="0.3">
@@ -13006,13 +13454,13 @@
         <v>24</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>1037</v>
+        <v>1055</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>1044</v>
+        <v>1062</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>1036</v>
+        <v>1054</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
@@ -13023,13 +13471,13 @@
         <v>25</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>1039</v>
+        <v>1057</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>1045</v>
+        <v>1063</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>1038</v>
+        <v>1056</v>
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
@@ -13040,13 +13488,13 @@
         <v>26</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>1042</v>
+        <v>1060</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>1040</v>
+        <v>1058</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>1041</v>
+        <v>1059</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -13057,13 +13505,13 @@
         <v>27</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>1046</v>
+        <v>1064</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>1047</v>
+        <v>1065</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>680</v>
+        <v>689</v>
       </c>
     </row>
     <row r="33" spans="5:8" x14ac:dyDescent="0.3">
@@ -13071,13 +13519,13 @@
         <v>28</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>1048</v>
+        <v>1066</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>1075</v>
+        <v>1093</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>1076</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="34" spans="5:8" x14ac:dyDescent="0.3">
@@ -13085,13 +13533,13 @@
         <v>29</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>1049</v>
+        <v>1067</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>1091</v>
+        <v>1109</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>1077</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="35" spans="5:8" x14ac:dyDescent="0.3">
@@ -13099,13 +13547,13 @@
         <v>30</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>1051</v>
+        <v>1069</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>1052</v>
+        <v>1070</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>1078</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="36" spans="5:8" x14ac:dyDescent="0.3">
@@ -13113,13 +13561,13 @@
         <v>31</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>1053</v>
+        <v>1071</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>1054</v>
+        <v>1072</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>1079</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="37" spans="5:8" x14ac:dyDescent="0.3">
@@ -13127,13 +13575,13 @@
         <v>32</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>1055</v>
+        <v>1073</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>1056</v>
+        <v>1074</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>1080</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="38" spans="5:8" x14ac:dyDescent="0.3">
@@ -13141,13 +13589,13 @@
         <v>33</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>1057</v>
+        <v>1075</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>1058</v>
+        <v>1076</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>1081</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="39" spans="5:8" x14ac:dyDescent="0.3">
@@ -13155,13 +13603,13 @@
         <v>34</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>1059</v>
+        <v>1077</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>1082</v>
+        <v>1100</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>1083</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="40" spans="5:8" x14ac:dyDescent="0.3">
@@ -13169,13 +13617,13 @@
         <v>35</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>1060</v>
+        <v>1078</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>1061</v>
+        <v>1079</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>1084</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="41" spans="5:8" x14ac:dyDescent="0.3">
@@ -13183,13 +13631,13 @@
         <v>36</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>1062</v>
+        <v>1080</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>1063</v>
+        <v>1081</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>1085</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="42" spans="5:8" x14ac:dyDescent="0.3">
@@ -13197,13 +13645,13 @@
         <v>37</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>1064</v>
+        <v>1082</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>1065</v>
+        <v>1083</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>1086</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="43" spans="5:8" x14ac:dyDescent="0.3">
@@ -13211,13 +13659,13 @@
         <v>38</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>1066</v>
+        <v>1084</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>1067</v>
+        <v>1085</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>1087</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="44" spans="5:8" x14ac:dyDescent="0.3">
@@ -13225,13 +13673,13 @@
         <v>39</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>1068</v>
+        <v>1086</v>
       </c>
       <c r="G44" s="4" t="s">
+        <v>1124</v>
+      </c>
+      <c r="H44" s="4" t="s">
         <v>1106</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>1088</v>
       </c>
     </row>
     <row r="45" spans="5:8" x14ac:dyDescent="0.3">
@@ -13239,13 +13687,13 @@
         <v>40</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>1069</v>
+        <v>1087</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>1070</v>
+        <v>1088</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>1089</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="46" spans="5:8" x14ac:dyDescent="0.3">
@@ -13253,13 +13701,13 @@
         <v>41</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>1090</v>
+        <v>1108</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>1127</v>
+        <v>1145</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>1128</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="47" spans="5:8" x14ac:dyDescent="0.3">
@@ -13267,13 +13715,13 @@
         <v>42</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>1093</v>
+        <v>1111</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>1092</v>
+        <v>1110</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>1129</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="48" spans="5:8" x14ac:dyDescent="0.3">
@@ -13281,13 +13729,13 @@
         <v>43</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>1094</v>
+        <v>1112</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>1095</v>
+        <v>1113</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>1130</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="49" spans="5:8" x14ac:dyDescent="0.3">
@@ -13295,13 +13743,13 @@
         <v>44</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>1096</v>
+        <v>1114</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>1131</v>
+        <v>1149</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>1132</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="50" spans="5:8" x14ac:dyDescent="0.3">
@@ -13309,13 +13757,13 @@
         <v>45</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>1097</v>
+        <v>1115</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>1098</v>
+        <v>1116</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>1133</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="51" spans="5:8" x14ac:dyDescent="0.3">
@@ -13323,13 +13771,13 @@
         <v>46</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>1099</v>
+        <v>1117</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>1100</v>
+        <v>1118</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>1134</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="52" spans="5:8" x14ac:dyDescent="0.3">
@@ -13337,13 +13785,13 @@
         <v>47</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>1102</v>
+        <v>1120</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>1101</v>
+        <v>1119</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>1135</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="53" spans="5:8" x14ac:dyDescent="0.3">
@@ -13351,13 +13799,13 @@
         <v>48</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>1103</v>
+        <v>1121</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>1104</v>
+        <v>1122</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>1136</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="54" spans="5:8" x14ac:dyDescent="0.3">
@@ -13365,13 +13813,13 @@
         <v>49</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>1105</v>
+        <v>1123</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>1137</v>
+        <v>1155</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>1138</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="55" spans="5:8" x14ac:dyDescent="0.3">
@@ -13379,13 +13827,13 @@
         <v>50</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>1107</v>
+        <v>1125</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>1139</v>
+        <v>1126</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>1140</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="56" spans="5:8" x14ac:dyDescent="0.3">
@@ -13393,13 +13841,13 @@
         <v>51</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>687</v>
+        <v>698</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>1108</v>
+        <v>1127</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>1141</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="57" spans="5:8" x14ac:dyDescent="0.3">
@@ -13407,13 +13855,13 @@
         <v>52</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>1109</v>
+        <v>1128</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>1142</v>
+        <v>1159</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>1143</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="58" spans="5:8" x14ac:dyDescent="0.3">
@@ -13421,13 +13869,13 @@
         <v>53</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>1144</v>
+        <v>1161</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>1110</v>
+        <v>1129</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>1145</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="59" spans="5:8" x14ac:dyDescent="0.3">
@@ -13435,13 +13883,13 @@
         <v>54</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>1111</v>
+        <v>1177</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>1146</v>
+        <v>1193</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>1147</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="60" spans="5:8" x14ac:dyDescent="0.3">
@@ -13449,13 +13897,13 @@
         <v>55</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>1112</v>
+        <v>1130</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>1113</v>
+        <v>1131</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>1148</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="61" spans="5:8" x14ac:dyDescent="0.3">
@@ -13463,13 +13911,13 @@
         <v>56</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>1114</v>
+        <v>1132</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>1115</v>
+        <v>1133</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>1149</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="62" spans="5:8" x14ac:dyDescent="0.3">
@@ -13477,13 +13925,13 @@
         <v>57</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>1116</v>
+        <v>1134</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>1117</v>
+        <v>1135</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>1150</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="63" spans="5:8" x14ac:dyDescent="0.3">
@@ -13491,13 +13939,13 @@
         <v>58</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>1118</v>
+        <v>1136</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>1119</v>
+        <v>1137</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>1151</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="64" spans="5:8" x14ac:dyDescent="0.3">
@@ -13505,13 +13953,13 @@
         <v>59</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>1120</v>
+        <v>1138</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>1121</v>
+        <v>1139</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>1152</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="65" spans="5:8" x14ac:dyDescent="0.3">
@@ -13519,13 +13967,13 @@
         <v>60</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>1122</v>
+        <v>1140</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>1123</v>
+        <v>1141</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>1153</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="66" spans="5:8" x14ac:dyDescent="0.3">
@@ -13533,13 +13981,13 @@
         <v>61</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>1124</v>
+        <v>1142</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>1159</v>
+        <v>1175</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>1154</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="67" spans="5:8" x14ac:dyDescent="0.3">
@@ -13547,13 +13995,13 @@
         <v>62</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>1125</v>
+        <v>1143</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>1155</v>
+        <v>1171</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>1156</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="68" spans="5:8" x14ac:dyDescent="0.3">
@@ -13561,358 +14009,616 @@
         <v>63</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>1126</v>
+        <v>1144</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>1157</v>
+        <v>1173</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>1158</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="69" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E69" s="4">
         <v>64</v>
       </c>
-      <c r="F69" s="4"/>
-      <c r="G69" s="4"/>
-      <c r="H69" s="6"/>
+      <c r="F69" s="4" t="s">
+        <v>1178</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>1179</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>1201</v>
+      </c>
     </row>
     <row r="70" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E70" s="4">
         <v>65</v>
       </c>
-      <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
-      <c r="H70" s="6"/>
+      <c r="F70" s="4" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>1181</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>1202</v>
+      </c>
     </row>
     <row r="71" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E71" s="4">
         <v>66</v>
       </c>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="6"/>
+      <c r="F71" s="4" t="s">
+        <v>1182</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>1183</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>1203</v>
+      </c>
     </row>
     <row r="72" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E72" s="4">
         <v>67</v>
       </c>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
-      <c r="H72" s="6"/>
+      <c r="F72" s="4" t="s">
+        <v>682</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>1184</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="73" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E73" s="4">
         <v>68</v>
       </c>
-      <c r="F73" s="4"/>
-      <c r="G73" s="4"/>
-      <c r="H73" s="6"/>
+      <c r="F73" s="4" t="s">
+        <v>1185</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>1186</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>1204</v>
+      </c>
     </row>
     <row r="74" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E74" s="4">
         <v>69</v>
       </c>
-      <c r="F74" s="4"/>
-      <c r="G74" s="4"/>
-      <c r="H74" s="6"/>
+      <c r="F74" s="4" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>1188</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>1205</v>
+      </c>
     </row>
     <row r="75" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E75" s="4">
         <v>70</v>
       </c>
-      <c r="F75" s="4"/>
-      <c r="G75" s="4"/>
-      <c r="H75" s="6"/>
+      <c r="F75" s="4" t="s">
+        <v>1191</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>1206</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>1207</v>
+      </c>
     </row>
     <row r="76" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E76" s="4">
         <v>71</v>
       </c>
-      <c r="F76" s="4"/>
-      <c r="G76" s="4"/>
-      <c r="H76" s="6"/>
+      <c r="F76" s="4" t="s">
+        <v>1189</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>1208</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>1209</v>
+      </c>
     </row>
     <row r="77" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E77" s="4">
         <v>72</v>
       </c>
-      <c r="F77" s="4"/>
-      <c r="G77" s="4"/>
-      <c r="H77" s="6"/>
+      <c r="F77" s="4" t="s">
+        <v>1190</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>1210</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>1211</v>
+      </c>
     </row>
     <row r="78" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E78" s="4">
         <v>73</v>
       </c>
-      <c r="F78" s="4"/>
-      <c r="G78" s="4"/>
-      <c r="H78" s="6"/>
+      <c r="F78" s="4" t="s">
+        <v>1192</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>1212</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>1213</v>
+      </c>
     </row>
     <row r="79" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E79" s="4">
         <v>74</v>
       </c>
-      <c r="F79" s="4"/>
-      <c r="G79" s="4"/>
-      <c r="H79" s="6"/>
+      <c r="F79" s="4" t="s">
+        <v>1214</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>1215</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>1216</v>
+      </c>
     </row>
     <row r="80" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E80" s="4">
         <v>75</v>
       </c>
-      <c r="F80" s="4"/>
-      <c r="G80" s="4"/>
-      <c r="H80" s="6"/>
+      <c r="F80" s="4" t="s">
+        <v>680</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>1194</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="81" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E81" s="4">
         <v>76</v>
       </c>
-      <c r="F81" s="4"/>
-      <c r="G81" s="4"/>
-      <c r="H81" s="6"/>
+      <c r="F81" s="4" t="s">
+        <v>1195</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>1217</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>1218</v>
+      </c>
     </row>
     <row r="82" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E82" s="4">
         <v>77</v>
       </c>
-      <c r="F82" s="4"/>
-      <c r="G82" s="4"/>
-      <c r="H82" s="6"/>
+      <c r="F82" s="4" t="s">
+        <v>1196</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>1197</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>686</v>
+      </c>
     </row>
     <row r="83" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E83" s="4">
         <v>78</v>
       </c>
-      <c r="F83" s="4"/>
-      <c r="G83" s="4"/>
-      <c r="H83" s="6"/>
+      <c r="F83" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H83" s="4" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="84" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E84" s="4">
         <v>79</v>
       </c>
-      <c r="F84" s="4"/>
-      <c r="G84" s="4"/>
-      <c r="H84" s="6"/>
+      <c r="F84" s="4" t="s">
+        <v>1198</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>1220</v>
+      </c>
+      <c r="H84" s="4" t="s">
+        <v>1221</v>
+      </c>
     </row>
     <row r="85" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E85" s="4">
         <v>80</v>
       </c>
-      <c r="F85" s="4"/>
-      <c r="G85" s="4"/>
-      <c r="H85" s="6"/>
+      <c r="F85" s="4" t="s">
+        <v>687</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>1222</v>
+      </c>
+      <c r="H85" s="4" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="86" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E86" s="4">
         <v>81</v>
       </c>
-      <c r="F86" s="4"/>
-      <c r="G86" s="4"/>
-      <c r="H86" s="6"/>
+      <c r="F86" s="4" t="s">
+        <v>1223</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>1233</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>1224</v>
+      </c>
     </row>
     <row r="87" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E87" s="4">
         <v>82</v>
       </c>
-      <c r="F87" s="4"/>
-      <c r="G87" s="4"/>
-      <c r="H87" s="6"/>
+      <c r="F87" s="4" t="s">
+        <v>1225</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>1199</v>
+      </c>
+      <c r="H87" s="4" t="s">
+        <v>1226</v>
+      </c>
     </row>
     <row r="88" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E88" s="4">
         <v>83</v>
       </c>
-      <c r="F88" s="4"/>
-      <c r="G88" s="4"/>
-      <c r="H88" s="6"/>
+      <c r="F88" s="4" t="s">
+        <v>1227</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>1200</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>1228</v>
+      </c>
     </row>
     <row r="89" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E89" s="4">
         <v>84</v>
       </c>
-      <c r="F89" s="4"/>
-      <c r="G89" s="4"/>
-      <c r="H89" s="6"/>
+      <c r="F89" s="4" t="s">
+        <v>1229</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>1230</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>1231</v>
+      </c>
     </row>
     <row r="90" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E90" s="4">
         <v>85</v>
       </c>
-      <c r="F90" s="4"/>
-      <c r="G90" s="4"/>
-      <c r="H90" s="6"/>
+      <c r="F90" s="4" t="s">
+        <v>1232</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>1259</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>1260</v>
+      </c>
     </row>
     <row r="91" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E91" s="4">
         <v>86</v>
       </c>
-      <c r="F91" s="4"/>
-      <c r="G91" s="4"/>
-      <c r="H91" s="6"/>
+      <c r="F91" s="4" t="s">
+        <v>1234</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>1261</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>1262</v>
+      </c>
     </row>
     <row r="92" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E92" s="4">
         <v>87</v>
       </c>
-      <c r="F92" s="4"/>
-      <c r="G92" s="4"/>
-      <c r="H92" s="4"/>
+      <c r="F92" s="4" t="s">
+        <v>1235</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>1263</v>
+      </c>
+      <c r="H92" s="4" t="s">
+        <v>1264</v>
+      </c>
     </row>
     <row r="93" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E93" s="4">
         <v>88</v>
       </c>
-      <c r="F93" s="4"/>
-      <c r="G93" s="4"/>
-      <c r="H93" s="4"/>
+      <c r="F93" s="4" t="s">
+        <v>1236</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>1237</v>
+      </c>
+      <c r="H93" s="4" t="s">
+        <v>1265</v>
+      </c>
     </row>
     <row r="94" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E94" s="4">
         <v>89</v>
       </c>
-      <c r="F94" s="4"/>
-      <c r="G94" s="4"/>
-      <c r="H94" s="4"/>
+      <c r="F94" s="4" t="s">
+        <v>1238</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>1266</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>1267</v>
+      </c>
     </row>
     <row r="95" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E95" s="4">
         <v>90</v>
       </c>
-      <c r="F95" s="4"/>
-      <c r="G95" s="4"/>
-      <c r="H95" s="4"/>
+      <c r="F95" s="4" t="s">
+        <v>1239</v>
+      </c>
+      <c r="G95" s="4" t="s">
+        <v>1240</v>
+      </c>
+      <c r="H95" s="4" t="s">
+        <v>1268</v>
+      </c>
     </row>
     <row r="96" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E96" s="4">
         <v>91</v>
       </c>
-      <c r="F96" s="4"/>
-      <c r="G96" s="4"/>
-      <c r="H96" s="4"/>
+      <c r="F96" s="4" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>1269</v>
+      </c>
+      <c r="H96" s="4" t="s">
+        <v>1270</v>
+      </c>
     </row>
     <row r="97" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E97" s="4">
         <v>92</v>
       </c>
-      <c r="F97" s="4"/>
-      <c r="G97" s="4"/>
-      <c r="H97" s="4"/>
+      <c r="F97" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="G97" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="H97" s="4" t="s">
+        <v>701</v>
+      </c>
     </row>
     <row r="98" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E98" s="4">
         <v>93</v>
       </c>
-      <c r="F98" s="4"/>
-      <c r="G98" s="4"/>
-      <c r="H98" s="4"/>
+      <c r="F98" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="G98" s="4" t="s">
+        <v>1272</v>
+      </c>
+      <c r="H98" s="4" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="99" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E99" s="4">
         <v>94</v>
       </c>
-      <c r="F99" s="4"/>
-      <c r="G99" s="4"/>
-      <c r="H99" s="4"/>
+      <c r="F99" s="4" t="s">
+        <v>1242</v>
+      </c>
+      <c r="G99" s="4" t="s">
+        <v>1273</v>
+      </c>
+      <c r="H99" s="4" t="s">
+        <v>1274</v>
+      </c>
     </row>
     <row r="100" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E100" s="4">
         <v>95</v>
       </c>
-      <c r="F100" s="4"/>
-      <c r="G100" s="4"/>
-      <c r="H100" s="4"/>
+      <c r="F100" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="G100" s="4" t="s">
+        <v>1243</v>
+      </c>
+      <c r="H100" s="4" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="101" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E101" s="4">
         <v>96</v>
       </c>
-      <c r="F101" s="4"/>
-      <c r="G101" s="4"/>
-      <c r="H101" s="4"/>
+      <c r="F101" s="4" t="s">
+        <v>1244</v>
+      </c>
+      <c r="G101" s="4" t="s">
+        <v>1276</v>
+      </c>
+      <c r="H101" s="4" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="102" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E102" s="4">
         <v>97</v>
       </c>
-      <c r="F102" s="4"/>
-      <c r="G102" s="4"/>
-      <c r="H102" s="4"/>
+      <c r="F102" s="4" t="s">
+        <v>1245</v>
+      </c>
+      <c r="G102" s="4" t="s">
+        <v>1246</v>
+      </c>
+      <c r="H102" s="4" t="s">
+        <v>1277</v>
+      </c>
     </row>
     <row r="103" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E103" s="4">
         <v>98</v>
       </c>
-      <c r="F103" s="4"/>
-      <c r="G103" s="4"/>
-      <c r="H103" s="4"/>
+      <c r="F103" s="4" t="s">
+        <v>1247</v>
+      </c>
+      <c r="G103" s="4" t="s">
+        <v>1278</v>
+      </c>
+      <c r="H103" s="4" t="s">
+        <v>1279</v>
+      </c>
     </row>
     <row r="104" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E104" s="4">
         <v>99</v>
       </c>
-      <c r="F104" s="4"/>
-      <c r="G104" s="4"/>
-      <c r="H104" s="4"/>
+      <c r="F104" s="4" t="s">
+        <v>690</v>
+      </c>
+      <c r="G104" s="4" t="s">
+        <v>1280</v>
+      </c>
+      <c r="H104" s="4" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="105" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E105" s="4">
         <v>100</v>
       </c>
-      <c r="F105" s="4"/>
-      <c r="G105" s="4"/>
-      <c r="H105" s="4"/>
+      <c r="F105" s="4" t="s">
+        <v>1248</v>
+      </c>
+      <c r="G105" s="4" t="s">
+        <v>1249</v>
+      </c>
+      <c r="H105" s="4" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="106" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E106" s="4">
         <v>101</v>
       </c>
-      <c r="F106" s="4"/>
-      <c r="G106" s="4"/>
-      <c r="H106" s="4"/>
+      <c r="F106" s="4" t="s">
+        <v>1250</v>
+      </c>
+      <c r="G106" s="4" t="s">
+        <v>1251</v>
+      </c>
+      <c r="H106" s="4" t="s">
+        <v>1281</v>
+      </c>
     </row>
     <row r="107" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E107" s="4">
         <v>102</v>
       </c>
-      <c r="F107" s="4"/>
-      <c r="G107" s="4"/>
-      <c r="H107" s="4"/>
+      <c r="F107" s="4" t="s">
+        <v>1252</v>
+      </c>
+      <c r="G107" s="4" t="s">
+        <v>1253</v>
+      </c>
+      <c r="H107" s="4" t="s">
+        <v>1282</v>
+      </c>
     </row>
     <row r="108" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E108" s="4">
         <v>103</v>
       </c>
-      <c r="F108" s="4"/>
-      <c r="G108" s="4"/>
-      <c r="H108" s="4"/>
+      <c r="F108" s="4" t="s">
+        <v>1254</v>
+      </c>
+      <c r="G108" s="4" t="s">
+        <v>1255</v>
+      </c>
+      <c r="H108" s="4" t="s">
+        <v>1283</v>
+      </c>
     </row>
     <row r="109" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E109" s="4">
         <v>104</v>
       </c>
-      <c r="F109" s="4"/>
-      <c r="G109" s="4"/>
-      <c r="H109" s="4"/>
+      <c r="F109" s="4" t="s">
+        <v>1256</v>
+      </c>
+      <c r="G109" s="4" t="s">
+        <v>1284</v>
+      </c>
+      <c r="H109" s="4" t="s">
+        <v>1285</v>
+      </c>
     </row>
     <row r="110" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E110" s="4">
         <v>105</v>
       </c>
-      <c r="F110" s="4"/>
-      <c r="G110" s="4"/>
-      <c r="H110" s="4"/>
+      <c r="F110" s="4" t="s">
+        <v>1257</v>
+      </c>
+      <c r="G110" s="4" t="s">
+        <v>1286</v>
+      </c>
+      <c r="H110" s="4" t="s">
+        <v>1287</v>
+      </c>
     </row>
     <row r="111" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E111" s="4">
         <v>106</v>
       </c>
-      <c r="F111" s="4"/>
-      <c r="G111" s="4"/>
-      <c r="H111" s="4"/>
+      <c r="F111" s="4" t="s">
+        <v>1258</v>
+      </c>
+      <c r="G111" s="4" t="s">
+        <v>1288</v>
+      </c>
+      <c r="H111" s="4" t="s">
+        <v>1289</v>
+      </c>
     </row>
     <row r="112" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E112" s="4">

</xml_diff>